<commit_message>
Se agregaron CU Reales Administrador
</commit_message>
<xml_diff>
--- a/Documentacion/CasosDeUso/Casos de uso real Administrador.xlsx
+++ b/Documentacion/CasosDeUso/Casos de uso real Administrador.xlsx
@@ -4,17 +4,25 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="441"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="615"/>
   </bookViews>
   <sheets>
-    <sheet name="PLANTILLA" sheetId="1" r:id="rId1"/>
+    <sheet name="CU Crear Historia Clinica" sheetId="11" r:id="rId1"/>
+    <sheet name="CU Deshabilitar Paciente" sheetId="10" r:id="rId2"/>
+    <sheet name="CU Deshabilitar Medico" sheetId="8" r:id="rId3"/>
+    <sheet name="CU Modificar Paciente" sheetId="7" r:id="rId4"/>
+    <sheet name="CU Modificar Medico" sheetId="6" r:id="rId5"/>
+    <sheet name="CU Consultar Paciente" sheetId="5" r:id="rId6"/>
+    <sheet name="CU Consultar Medico" sheetId="4" r:id="rId7"/>
+    <sheet name="CU Agregar Paciente" sheetId="3" r:id="rId8"/>
+    <sheet name="CU Agregar Medico" sheetId="1" r:id="rId9"/>
   </sheets>
   <calcPr calcId="125725" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="88">
   <si>
     <t>RFH-001</t>
   </si>
@@ -1662,1174 +1670,2521 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C3:F166"/>
+  <dimension ref="C2:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D158" sqref="D158"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="4" width="10.7109375"/>
-    <col min="5" max="5" width="48.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="48.140625" style="1"/>
+    <col min="3" max="3" width="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="46.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="48" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:6" ht="15.75" thickBot="1"/>
+    <row r="3" spans="3:6">
+      <c r="C3">
+        <v>9</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="3:6">
+      <c r="E4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="3:6">
+      <c r="E5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="3:6" ht="30">
+      <c r="E6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="3:6">
+      <c r="E7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="3:6">
+      <c r="E8" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="3:6">
+      <c r="E9" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="26"/>
+    </row>
+    <row r="10" spans="3:6">
+      <c r="E10" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="3:6" ht="45">
+      <c r="E11" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="3:6" ht="30">
+      <c r="E12" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="3:6" ht="30">
+      <c r="E13" s="15"/>
+      <c r="F13" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="3:6" ht="30">
+      <c r="E14" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="3:6" ht="30">
+      <c r="E15" s="15"/>
+      <c r="F15" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="3:6" ht="30">
+      <c r="E16" s="15"/>
+      <c r="F16" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="5:6">
+      <c r="E17" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="5:6" ht="60">
+      <c r="E18" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="5:6" ht="105.75" thickBot="1">
+      <c r="E19" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E9:F9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="C2:F38"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="46.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="48" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:6" ht="15.75" thickBot="1"/>
+    <row r="3" spans="3:6">
+      <c r="C3">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="3:6">
+      <c r="E4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="3:6">
+      <c r="E5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="3:6" ht="30">
+      <c r="E6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="3:6">
+      <c r="E7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="3:6">
+      <c r="E8" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="3:6">
+      <c r="E9" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="26"/>
+    </row>
+    <row r="10" spans="3:6">
+      <c r="E10" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="3:6" ht="45">
+      <c r="E11" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="3:6" ht="30">
+      <c r="E12" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="3:6" ht="30">
+      <c r="E13" s="15"/>
+      <c r="F13" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="3:6" ht="30">
+      <c r="E14" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="3:6" ht="30">
+      <c r="E15" s="15"/>
+      <c r="F15" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="3:6" ht="30">
+      <c r="E16" s="15"/>
+      <c r="F16" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6">
+      <c r="E17" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="24" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" ht="60">
+      <c r="E18" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="3:6" ht="105.75" thickBot="1">
+      <c r="E19" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="3:6" ht="15.75" thickBot="1"/>
+    <row r="22" spans="3:6">
+      <c r="C22">
+        <v>9</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="3:6">
+      <c r="E23" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="3:6">
+      <c r="E24" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="3:6" ht="30">
+      <c r="E25" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="3:6">
+      <c r="E26" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="3:6">
+      <c r="E27" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="3:6">
+      <c r="E28" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="F28" s="26"/>
+    </row>
+    <row r="29" spans="3:6">
+      <c r="E29" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="3:6" ht="45">
+      <c r="E30" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="F30" s="14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="3:6" ht="30">
+      <c r="E31" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F31" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="3:6" ht="30">
+      <c r="E32" s="15"/>
+      <c r="F32" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="5:6" ht="30">
+      <c r="E33" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="5:6" ht="30">
+      <c r="E34" s="15"/>
+      <c r="F34" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="5:6" ht="30">
+      <c r="E35" s="15"/>
+      <c r="F35" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="5:6">
+      <c r="E36" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F36" s="24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="5:6" ht="60">
+      <c r="E37" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="38" spans="5:6" ht="105.75" thickBot="1">
+      <c r="E38" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" s="23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E28:F28"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="C2:F19"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="46.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="48" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:6" ht="15.75" thickBot="1"/>
+    <row r="3" spans="3:6">
+      <c r="C3">
+        <v>7</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="3:6">
+      <c r="E4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="3:6">
+      <c r="E5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="3:6" ht="30">
+      <c r="E6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="3:6">
+      <c r="E7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="3:6">
+      <c r="E8" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="3:6">
+      <c r="E9" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="26"/>
+    </row>
+    <row r="10" spans="3:6">
+      <c r="E10" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="3:6" ht="45">
+      <c r="E11" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="3:6" ht="30">
+      <c r="E12" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="3:6" ht="30">
+      <c r="E13" s="15"/>
+      <c r="F13" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="3:6" ht="30">
+      <c r="E14" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="3:6" ht="30">
+      <c r="E15" s="15"/>
+      <c r="F15" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="3:6" ht="30">
+      <c r="E16" s="15"/>
+      <c r="F16" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="5:6">
+      <c r="E17" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="24" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="5:6" ht="60">
+      <c r="E18" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="5:6" ht="105.75" thickBot="1">
+      <c r="E19" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E9:F9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="C2:F20"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="46.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="48" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:6" ht="15.75" thickBot="1"/>
+    <row r="3" spans="3:6">
+      <c r="C3">
+        <v>6</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="3:6">
+      <c r="E4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="3:6">
+      <c r="E5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="3:6" ht="45">
+      <c r="E6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="3:6">
+      <c r="E7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="3:6">
+      <c r="E8" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="3:6">
+      <c r="E9" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="26"/>
+    </row>
+    <row r="10" spans="3:6">
+      <c r="E10" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="3:6" ht="45">
+      <c r="E11" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="3:6" ht="30">
+      <c r="E12" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="3:6" ht="30">
+      <c r="E13" s="15"/>
+      <c r="F13" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="3:6" ht="30">
+      <c r="E14" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="3:6" ht="30">
+      <c r="E15" s="15"/>
+      <c r="F15" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="3:6" ht="45">
+      <c r="E16" s="15"/>
+      <c r="F16" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="5:6" ht="30">
+      <c r="E17" s="15"/>
+      <c r="F17" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="5:6">
+      <c r="E18" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="24" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="5:6" ht="105">
+      <c r="E19" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="5:6" ht="105.75" thickBot="1">
+      <c r="E20" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E9:F9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="C2:F20"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="46.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="48" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:6" ht="15.75" thickBot="1"/>
+    <row r="3" spans="3:6">
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="3:6">
+      <c r="E4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="3:6">
+      <c r="E5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="3:6" ht="45">
+      <c r="E6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="3:6">
+      <c r="E7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="3:6">
+      <c r="E8" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="3:6">
+      <c r="E9" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="26"/>
+    </row>
+    <row r="10" spans="3:6">
+      <c r="E10" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="3:6" ht="45">
+      <c r="E11" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="3:6" ht="30">
+      <c r="E12" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="3:6" ht="30">
+      <c r="E13" s="15"/>
+      <c r="F13" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="3:6" ht="30">
+      <c r="E14" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="3:6" ht="30">
+      <c r="E15" s="15"/>
+      <c r="F15" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="3:6" ht="45">
+      <c r="E16" s="15"/>
+      <c r="F16" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="5:6" ht="30">
+      <c r="E17" s="15"/>
+      <c r="F17" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="5:6">
+      <c r="E18" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="24" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="5:6" ht="105">
+      <c r="E19" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="5:6" ht="105.75" thickBot="1">
+      <c r="E20" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E9:F9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="C2:F16"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="46.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="48" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:6" ht="15.75" thickBot="1"/>
+    <row r="3" spans="3:6">
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="3:6">
+      <c r="E4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="3:6">
+      <c r="E5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="3:6">
+      <c r="E6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="3:6">
+      <c r="E7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="3:6">
+      <c r="E8" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="3:6">
+      <c r="E9" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="26"/>
+    </row>
+    <row r="10" spans="3:6">
+      <c r="E10" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="3:6" ht="45">
+      <c r="E11" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="3:6" ht="30">
+      <c r="E12" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="3:6" ht="30">
+      <c r="E13" s="15"/>
+      <c r="F13" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="3:6">
+      <c r="E14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="3:6" ht="60">
+      <c r="E15" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="3:6" ht="105.75" thickBot="1">
+      <c r="E16" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E9:F9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="C2:F16"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="47.85546875" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:6" ht="15.75" thickBot="1"/>
+    <row r="3" spans="3:6">
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="3:6">
+      <c r="E4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="3:6">
+      <c r="E5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="3:6" ht="30">
+      <c r="E6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="3:6">
+      <c r="E7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="3:6">
+      <c r="E8" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="3:6">
+      <c r="E9" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="26"/>
+    </row>
+    <row r="10" spans="3:6">
+      <c r="E10" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="3:6" ht="45">
+      <c r="E11" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="3:6" ht="30">
+      <c r="E12" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="3:6" ht="30">
+      <c r="E13" s="15"/>
+      <c r="F13" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="3:6">
+      <c r="E14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="3:6" ht="60">
+      <c r="E15" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="3:6" ht="105.75" thickBot="1">
+      <c r="E16" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E9:F9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="C2:F18"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="41.5703125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:6" ht="15.75" thickBot="1"/>
+    <row r="3" spans="3:6">
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="3:6">
+      <c r="E4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="3:6">
+      <c r="E5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="3:6" ht="30">
+      <c r="E6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="3:6">
+      <c r="E7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="3:6">
+      <c r="E8" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="3:6">
+      <c r="E9" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="26"/>
+    </row>
+    <row r="10" spans="3:6">
+      <c r="E10" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="3:6" ht="45">
+      <c r="E11" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="3:6" ht="30">
+      <c r="E12" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="3:6" ht="30">
+      <c r="E13" s="15"/>
+      <c r="F13" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="3:6" ht="60">
+      <c r="E14" s="15"/>
+      <c r="F14" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="3:6" ht="30">
+      <c r="E15" s="16"/>
+      <c r="F15" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="3:6">
+      <c r="E16" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="5:6" ht="90">
+      <c r="E17" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="5:6" ht="135.75" thickBot="1">
+      <c r="E18" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E9:F9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="C2:F165"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="10.7109375"/>
+    <col min="3" max="3" width="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375"/>
+    <col min="5" max="5" width="46.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="48" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="1025" width="10.7109375"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:6" ht="15.75" thickBot="1"/>
+    <row r="2" spans="3:6" ht="15.75" thickBot="1"/>
+    <row r="3" spans="3:6">
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
     <row r="4" spans="3:6">
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>79</v>
+      <c r="E4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="3:6">
       <c r="E5" s="4" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="3:6">
-      <c r="E6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="3:6" ht="30">
+    <row r="6" spans="3:6" ht="30">
+      <c r="E6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="3:6">
       <c r="E7" s="6" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="3:6">
-      <c r="E8" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>14</v>
+      <c r="E8" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="3:6">
-      <c r="E9" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="3:6" ht="14.85" customHeight="1">
-      <c r="E10" s="25" t="s">
+      <c r="E9" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="F10" s="26"/>
-    </row>
-    <row r="11" spans="3:6">
-      <c r="E11" s="10" t="s">
+      <c r="F9" s="26"/>
+    </row>
+    <row r="10" spans="3:6">
+      <c r="E10" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F10" s="11" t="s">
         <v>6</v>
       </c>
     </row>
+    <row r="11" spans="3:6" ht="30">
+      <c r="E11" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
     <row r="12" spans="3:6" ht="30">
-      <c r="E12" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="3:6" ht="30">
-      <c r="E13" s="4" t="s">
+      <c r="E12" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="F12" s="14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="3:6">
+    <row r="13" spans="3:6">
+      <c r="E13" s="15"/>
+      <c r="F13" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="3:6" ht="45">
       <c r="E14" s="15"/>
       <c r="F14" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="3:6" ht="45">
-      <c r="E15" s="15"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="3:6" ht="30">
+      <c r="E15" s="16"/>
       <c r="F15" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="3:6" ht="30">
-      <c r="E16" s="16"/>
-      <c r="F16" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="3:6">
-      <c r="E17" s="6" t="s">
+    <row r="16" spans="3:6">
+      <c r="E16" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F16" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="3:6" ht="60">
-      <c r="E18" s="17" t="s">
+    <row r="17" spans="3:6" ht="60">
+      <c r="E17" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="F17" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="3:6" ht="105.75" thickBot="1">
-      <c r="E19" s="18" t="s">
+    <row r="18" spans="3:6" ht="105.75" thickBot="1">
+      <c r="E18" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="19" t="s">
+      <c r="F18" s="19" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="3:6" ht="15.75" thickBot="1"/>
+    <row r="20" spans="3:6" ht="15.75" thickBot="1"/>
+    <row r="21" spans="3:6">
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
     <row r="22" spans="3:6">
-      <c r="C22">
-        <v>2</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>80</v>
+      <c r="E22" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="3:6">
       <c r="E23" s="4" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="3:6">
-      <c r="E24" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F24" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="3:6" ht="30">
+    <row r="24" spans="3:6" ht="30">
+      <c r="E24" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="3:6">
       <c r="E25" s="6" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="3:6">
-      <c r="E26" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>14</v>
+      <c r="E26" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="3:6">
-      <c r="E27" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="F27" s="9" t="s">
-        <v>15</v>
-      </c>
+      <c r="E27" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27" s="21"/>
     </row>
     <row r="28" spans="3:6">
-      <c r="E28" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="F28" s="21"/>
-    </row>
-    <row r="29" spans="3:6">
-      <c r="E29" s="10" t="s">
+      <c r="E28" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F29" s="11" t="s">
+      <c r="F28" s="11" t="s">
         <v>6</v>
       </c>
     </row>
+    <row r="29" spans="3:6" ht="30">
+      <c r="E29" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F29" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
     <row r="30" spans="3:6" ht="30">
-      <c r="E30" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F30" s="13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="31" spans="3:6" ht="30">
-      <c r="E31" s="4" t="s">
+      <c r="E30" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F31" s="14" t="s">
+      <c r="F30" s="14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="3:6">
+    <row r="31" spans="3:6">
+      <c r="E31" s="15"/>
+      <c r="F31" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="3:6" ht="45">
       <c r="E32" s="15"/>
       <c r="F32" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="33" spans="3:6" ht="45">
-      <c r="E33" s="15"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="3:6" ht="30">
+      <c r="E33" s="16"/>
       <c r="F33" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="34" spans="3:6" ht="30">
-      <c r="E34" s="16"/>
-      <c r="F34" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="3:6">
-      <c r="E35" s="6" t="s">
+    <row r="34" spans="3:6">
+      <c r="E34" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F35" s="7" t="s">
+      <c r="F34" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="3:6" ht="60">
-      <c r="E36" s="17" t="s">
+    <row r="35" spans="3:6" ht="60">
+      <c r="E35" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="F36" s="5" t="s">
+      <c r="F35" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="3:6" ht="105.75" thickBot="1">
-      <c r="E37" s="18" t="s">
+    <row r="36" spans="3:6" ht="105.75" thickBot="1">
+      <c r="E36" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="F37" s="19" t="s">
+      <c r="F36" s="19" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="3:6" ht="15.75" thickBot="1"/>
+    <row r="38" spans="3:6" ht="15.75" thickBot="1"/>
+    <row r="39" spans="3:6">
+      <c r="C39">
+        <v>3</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
     <row r="40" spans="3:6">
-      <c r="C40">
-        <v>3</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>81</v>
+      <c r="E40" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="41" spans="3:6">
       <c r="E41" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="42" spans="3:6" ht="30">
+      <c r="E42" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" spans="3:6">
+      <c r="E43" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="3:6">
+      <c r="E44" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F44" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="3:6">
+      <c r="E45" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="F45" s="26"/>
+    </row>
+    <row r="46" spans="3:6">
+      <c r="E46" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F46" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="3:6" ht="45">
+      <c r="E47" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="F47" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="48" spans="3:6" ht="30">
+      <c r="E48" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F48" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="49" spans="3:6" ht="30">
+      <c r="E49" s="15"/>
+      <c r="F49" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="50" spans="3:6">
+      <c r="E50" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="51" spans="3:6" ht="60">
+      <c r="E51" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="52" spans="3:6" ht="105.75" thickBot="1">
+      <c r="E52" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F52" s="19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="54" spans="3:6" ht="15.75" thickBot="1"/>
+    <row r="55" spans="3:6">
+      <c r="C55">
+        <v>4</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="56" spans="3:6">
+      <c r="E56" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F41" s="5" t="s">
+      <c r="F56" s="5" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="42" spans="3:6">
-      <c r="E42" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="43" spans="3:6" ht="30">
-      <c r="E43" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="F43" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="44" spans="3:6">
-      <c r="E44" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F44" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="45" spans="3:6">
-      <c r="E45" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="F45" s="9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="46" spans="3:6">
-      <c r="E46" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="F46" s="26"/>
-    </row>
-    <row r="47" spans="3:6">
-      <c r="E47" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="F47" s="11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="48" spans="3:6" ht="45">
-      <c r="E48" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="F48" s="14" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="49" spans="3:6" ht="30">
-      <c r="E49" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F49" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="50" spans="3:6" ht="30">
-      <c r="E50" s="15"/>
-      <c r="F50" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="51" spans="3:6">
-      <c r="E51" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F51" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="52" spans="3:6" ht="60">
-      <c r="E52" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="53" spans="3:6" ht="105.75" thickBot="1">
-      <c r="E53" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F53" s="19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="55" spans="3:6" ht="15.75" thickBot="1"/>
-    <row r="56" spans="3:6">
-      <c r="C56">
-        <v>4</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F56" s="3" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="57" spans="3:6">
       <c r="E57" s="4" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
     </row>
     <row r="58" spans="3:6">
-      <c r="E58" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F58" s="5" t="s">
-        <v>31</v>
+      <c r="E58" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F58" s="7" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="59" spans="3:6">
       <c r="E59" s="6" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
     </row>
     <row r="60" spans="3:6">
-      <c r="E60" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F60" s="7" t="s">
-        <v>14</v>
+      <c r="E60" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F60" s="9" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="61" spans="3:6">
-      <c r="E61" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="F61" s="9" t="s">
-        <v>42</v>
-      </c>
+      <c r="E61" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="F61" s="26"/>
     </row>
     <row r="62" spans="3:6">
-      <c r="E62" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="F62" s="26"/>
-    </row>
-    <row r="63" spans="3:6">
-      <c r="E63" s="10" t="s">
+      <c r="E62" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F63" s="11" t="s">
+      <c r="F62" s="11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="3:6" ht="45">
-      <c r="E64" s="22" t="s">
+    <row r="63" spans="3:6" ht="45">
+      <c r="E63" s="22" t="s">
         <v>34</v>
       </c>
+      <c r="F63" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="64" spans="3:6" ht="30">
+      <c r="E64" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="F64" s="14" t="s">
-        <v>64</v>
+        <v>17</v>
       </c>
     </row>
     <row r="65" spans="3:6" ht="30">
-      <c r="E65" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F65" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="66" spans="3:6" ht="30">
-      <c r="E66" s="15"/>
-      <c r="F66" s="5" t="s">
+      <c r="E65" s="15"/>
+      <c r="F65" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="67" spans="3:6">
-      <c r="E67" s="6" t="s">
+    <row r="66" spans="3:6">
+      <c r="E66" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F67" s="7" t="s">
+      <c r="F66" s="7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="68" spans="3:6" ht="60">
-      <c r="E68" s="17" t="s">
+    <row r="67" spans="3:6" ht="60">
+      <c r="E67" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="F68" s="5" t="s">
+      <c r="F67" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="69" spans="3:6" ht="105.75" thickBot="1">
-      <c r="E69" s="18" t="s">
+    <row r="68" spans="3:6" ht="105.75" thickBot="1">
+      <c r="E68" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="F69" s="23" t="s">
+      <c r="F68" s="23" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="71" spans="3:6" ht="15.75" thickBot="1"/>
+    <row r="70" spans="3:6" ht="15.75" thickBot="1"/>
+    <row r="71" spans="3:6">
+      <c r="C71">
+        <v>5</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F71" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
     <row r="72" spans="3:6">
-      <c r="C72">
-        <v>5</v>
-      </c>
-      <c r="E72" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F72" s="3" t="s">
-        <v>83</v>
+      <c r="E72" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F72" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="73" spans="3:6">
       <c r="E73" s="4" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="74" spans="3:6">
-      <c r="E74" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F74" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="75" spans="3:6" ht="45">
+    <row r="74" spans="3:6" ht="45">
+      <c r="E74" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F74" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="75" spans="3:6">
       <c r="E75" s="6" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F75" s="7" t="s">
-        <v>56</v>
+        <v>14</v>
       </c>
     </row>
     <row r="76" spans="3:6">
-      <c r="E76" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F76" s="7" t="s">
-        <v>14</v>
+      <c r="E76" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F76" s="9" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="77" spans="3:6">
-      <c r="E77" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="F77" s="9" t="s">
-        <v>33</v>
-      </c>
+      <c r="E77" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="F77" s="26"/>
     </row>
     <row r="78" spans="3:6">
-      <c r="E78" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="F78" s="26"/>
-    </row>
-    <row r="79" spans="3:6">
-      <c r="E79" s="10" t="s">
+      <c r="E78" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F79" s="11" t="s">
+      <c r="F78" s="11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="3:6" ht="45">
-      <c r="E80" s="22" t="s">
+    <row r="79" spans="3:6" ht="45">
+      <c r="E79" s="22" t="s">
         <v>34</v>
       </c>
+      <c r="F79" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="80" spans="3:6" ht="30">
+      <c r="E80" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="F80" s="14" t="s">
-        <v>64</v>
+        <v>17</v>
       </c>
     </row>
     <row r="81" spans="3:6" ht="30">
-      <c r="E81" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F81" s="14" t="s">
-        <v>17</v>
+      <c r="E81" s="15"/>
+      <c r="F81" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="82" spans="3:6" ht="30">
-      <c r="E82" s="15"/>
-      <c r="F82" s="5" t="s">
-        <v>36</v>
+      <c r="E82" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="F82" s="14" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="83" spans="3:6" ht="30">
-      <c r="E83" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="F83" s="14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="84" spans="3:6" ht="30">
+      <c r="E83" s="15"/>
+      <c r="F83" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="84" spans="3:6" ht="45">
       <c r="E84" s="15"/>
       <c r="F84" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="85" spans="3:6" ht="45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="85" spans="3:6" ht="30">
       <c r="E85" s="15"/>
       <c r="F85" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="86" spans="3:6" ht="30">
-      <c r="E86" s="15"/>
-      <c r="F86" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="87" spans="3:6">
-      <c r="E87" s="6" t="s">
+    <row r="86" spans="3:6">
+      <c r="E86" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F87" s="24" t="s">
+      <c r="F86" s="24" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="88" spans="3:6" ht="105">
-      <c r="E88" s="17" t="s">
+    <row r="87" spans="3:6" ht="105">
+      <c r="E87" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="F88" s="5" t="s">
+      <c r="F87" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="89" spans="3:6" ht="105.75" thickBot="1">
-      <c r="E89" s="18" t="s">
+    <row r="88" spans="3:6" ht="105.75" thickBot="1">
+      <c r="E88" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="F89" s="23" t="s">
+      <c r="F88" s="23" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="91" spans="3:6" ht="15.75" thickBot="1"/>
+    <row r="90" spans="3:6" ht="15.75" thickBot="1"/>
+    <row r="91" spans="3:6">
+      <c r="C91">
+        <v>6</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F91" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
     <row r="92" spans="3:6">
-      <c r="C92">
-        <v>6</v>
-      </c>
-      <c r="E92" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F92" s="3" t="s">
-        <v>84</v>
+      <c r="E92" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F92" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="93" spans="3:6">
       <c r="E93" s="4" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="F93" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="94" spans="3:6">
-      <c r="E94" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F94" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="95" spans="3:6" ht="45">
+    <row r="94" spans="3:6" ht="45">
+      <c r="E94" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F94" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="95" spans="3:6">
       <c r="E95" s="6" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F95" s="7" t="s">
-        <v>55</v>
+        <v>14</v>
       </c>
     </row>
     <row r="96" spans="3:6">
-      <c r="E96" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F96" s="7" t="s">
-        <v>14</v>
+      <c r="E96" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F96" s="9" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="97" spans="3:6">
-      <c r="E97" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="F97" s="9" t="s">
-        <v>40</v>
-      </c>
+      <c r="E97" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="F97" s="26"/>
     </row>
     <row r="98" spans="3:6">
-      <c r="E98" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="F98" s="26"/>
-    </row>
-    <row r="99" spans="3:6">
-      <c r="E99" s="10" t="s">
+      <c r="E98" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F99" s="11" t="s">
+      <c r="F98" s="11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="100" spans="3:6" ht="45">
-      <c r="E100" s="22" t="s">
+    <row r="99" spans="3:6" ht="45">
+      <c r="E99" s="22" t="s">
         <v>34</v>
       </c>
+      <c r="F99" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="100" spans="3:6" ht="30">
+      <c r="E100" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="F100" s="14" t="s">
-        <v>64</v>
+        <v>17</v>
       </c>
     </row>
     <row r="101" spans="3:6" ht="30">
-      <c r="E101" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F101" s="14" t="s">
-        <v>17</v>
+      <c r="E101" s="15"/>
+      <c r="F101" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="102" spans="3:6" ht="30">
-      <c r="E102" s="15"/>
-      <c r="F102" s="5" t="s">
-        <v>41</v>
+      <c r="E102" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="F102" s="14" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="103" spans="3:6" ht="30">
-      <c r="E103" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="F103" s="14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="104" spans="3:6" ht="30">
+      <c r="E103" s="15"/>
+      <c r="F103" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="104" spans="3:6" ht="45">
       <c r="E104" s="15"/>
       <c r="F104" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="105" spans="3:6" ht="45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="105" spans="3:6" ht="30">
       <c r="E105" s="15"/>
       <c r="F105" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="106" spans="3:6" ht="30">
-      <c r="E106" s="15"/>
-      <c r="F106" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="107" spans="3:6">
-      <c r="E107" s="6" t="s">
+    <row r="106" spans="3:6">
+      <c r="E106" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F107" s="24" t="s">
+      <c r="F106" s="24" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="108" spans="3:6" ht="105">
-      <c r="E108" s="17" t="s">
+    <row r="107" spans="3:6" ht="105">
+      <c r="E107" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="F108" s="5" t="s">
+      <c r="F107" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="109" spans="3:6" ht="105.75" thickBot="1">
-      <c r="E109" s="18" t="s">
+    <row r="108" spans="3:6" ht="105.75" thickBot="1">
+      <c r="E108" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="F109" s="23" t="s">
+      <c r="F108" s="23" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="111" spans="3:6" ht="15.75" thickBot="1"/>
+    <row r="110" spans="3:6" ht="15.75" thickBot="1"/>
+    <row r="111" spans="3:6">
+      <c r="C111">
+        <v>7</v>
+      </c>
+      <c r="E111" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F111" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
     <row r="112" spans="3:6">
-      <c r="C112">
-        <v>7</v>
-      </c>
-      <c r="E112" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F112" s="3" t="s">
-        <v>85</v>
+      <c r="E112" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F112" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="113" spans="5:6">
       <c r="E113" s="4" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="F113" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="114" spans="5:6">
-      <c r="E114" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F114" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="115" spans="5:6" ht="30">
+    <row r="114" spans="5:6" ht="30">
+      <c r="E114" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F114" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="115" spans="5:6">
       <c r="E115" s="6" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F115" s="7" t="s">
-        <v>72</v>
+        <v>14</v>
       </c>
     </row>
     <row r="116" spans="5:6">
-      <c r="E116" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F116" s="7" t="s">
-        <v>14</v>
+      <c r="E116" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F116" s="9" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="117" spans="5:6">
-      <c r="E117" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="F117" s="9" t="s">
-        <v>33</v>
-      </c>
+      <c r="E117" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="F117" s="26"/>
     </row>
     <row r="118" spans="5:6">
-      <c r="E118" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="F118" s="26"/>
-    </row>
-    <row r="119" spans="5:6">
-      <c r="E119" s="10" t="s">
+      <c r="E118" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F119" s="11" t="s">
+      <c r="F118" s="11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="120" spans="5:6" ht="45">
-      <c r="E120" s="22" t="s">
+    <row r="119" spans="5:6" ht="45">
+      <c r="E119" s="22" t="s">
         <v>34</v>
       </c>
+      <c r="F119" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="120" spans="5:6" ht="30">
+      <c r="E120" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="F120" s="14" t="s">
-        <v>64</v>
+        <v>17</v>
       </c>
     </row>
     <row r="121" spans="5:6" ht="30">
-      <c r="E121" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F121" s="14" t="s">
-        <v>17</v>
+      <c r="E121" s="15"/>
+      <c r="F121" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="122" spans="5:6" ht="30">
-      <c r="E122" s="15"/>
+      <c r="E122" s="12" t="s">
+        <v>57</v>
+      </c>
       <c r="F122" s="5" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="123" spans="5:6" ht="30">
-      <c r="E123" s="12" t="s">
-        <v>57</v>
-      </c>
+      <c r="E123" s="15"/>
       <c r="F123" s="5" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
     </row>
     <row r="124" spans="5:6" ht="30">
       <c r="E124" s="15"/>
       <c r="F124" s="5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="125" spans="5:6" ht="30">
-      <c r="E125" s="15"/>
-      <c r="F125" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="126" spans="5:6">
-      <c r="E126" s="6" t="s">
+    <row r="125" spans="5:6">
+      <c r="E125" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F126" s="24" t="s">
+      <c r="F125" s="24" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="127" spans="5:6" ht="60">
-      <c r="E127" s="17" t="s">
+    <row r="126" spans="5:6" ht="60">
+      <c r="E126" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="F127" s="5" t="s">
+      <c r="F126" s="5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="128" spans="5:6" ht="105.75" thickBot="1">
-      <c r="E128" s="18" t="s">
+    <row r="127" spans="5:6" ht="105.75" thickBot="1">
+      <c r="E127" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="F128" s="23" t="s">
+      <c r="F127" s="23" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="130" spans="3:6" ht="15.75" thickBot="1"/>
+    <row r="129" spans="3:6" ht="15.75" thickBot="1"/>
+    <row r="130" spans="3:6">
+      <c r="C130">
+        <v>8</v>
+      </c>
+      <c r="E130" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F130" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
     <row r="131" spans="3:6">
-      <c r="C131">
-        <v>8</v>
-      </c>
-      <c r="E131" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F131" s="3" t="s">
-        <v>86</v>
+      <c r="E131" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F131" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="132" spans="3:6">
       <c r="E132" s="4" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="F132" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="133" spans="3:6">
-      <c r="E133" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F133" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="134" spans="3:6" ht="30">
+    <row r="133" spans="3:6" ht="30">
+      <c r="E133" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F133" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="134" spans="3:6">
       <c r="E134" s="6" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F134" s="7" t="s">
-        <v>75</v>
+        <v>14</v>
       </c>
     </row>
     <row r="135" spans="3:6">
-      <c r="E135" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F135" s="7" t="s">
-        <v>14</v>
+      <c r="E135" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F135" s="9" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="136" spans="3:6">
-      <c r="E136" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="F136" s="9" t="s">
-        <v>40</v>
-      </c>
+      <c r="E136" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="F136" s="26"/>
     </row>
     <row r="137" spans="3:6">
-      <c r="E137" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="F137" s="26"/>
-    </row>
-    <row r="138" spans="3:6">
-      <c r="E138" s="10" t="s">
+      <c r="E137" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F138" s="11" t="s">
+      <c r="F137" s="11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="139" spans="3:6" ht="45">
-      <c r="E139" s="22" t="s">
+    <row r="138" spans="3:6" ht="45">
+      <c r="E138" s="22" t="s">
         <v>34</v>
       </c>
+      <c r="F138" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="139" spans="3:6" ht="30">
+      <c r="E139" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="F139" s="14" t="s">
-        <v>64</v>
+        <v>17</v>
       </c>
     </row>
     <row r="140" spans="3:6" ht="30">
-      <c r="E140" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F140" s="14" t="s">
-        <v>17</v>
+      <c r="E140" s="15"/>
+      <c r="F140" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="141" spans="3:6" ht="30">
-      <c r="E141" s="15"/>
+      <c r="E141" s="12" t="s">
+        <v>77</v>
+      </c>
       <c r="F141" s="5" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
     </row>
     <row r="142" spans="3:6" ht="30">
-      <c r="E142" s="12" t="s">
-        <v>77</v>
-      </c>
+      <c r="E142" s="15"/>
       <c r="F142" s="5" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
     </row>
     <row r="143" spans="3:6" ht="30">
       <c r="E143" s="15"/>
       <c r="F143" s="5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="144" spans="3:6" ht="30">
-      <c r="E144" s="15"/>
-      <c r="F144" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="145" spans="3:6">
-      <c r="E145" s="6" t="s">
+    <row r="144" spans="3:6">
+      <c r="E144" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F145" s="24" t="s">
+      <c r="F144" s="24" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="146" spans="3:6" ht="60">
-      <c r="E146" s="17" t="s">
+    <row r="145" spans="3:6" ht="60">
+      <c r="E145" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="F146" s="5" t="s">
+      <c r="F145" s="5" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="147" spans="3:6" ht="105.75" thickBot="1">
-      <c r="E147" s="18" t="s">
+    <row r="146" spans="3:6" ht="105.75" thickBot="1">
+      <c r="E146" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="F147" s="23" t="s">
+      <c r="F146" s="23" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="149" spans="3:6" ht="15.75" thickBot="1"/>
+    <row r="148" spans="3:6" ht="15.75" thickBot="1"/>
+    <row r="149" spans="3:6">
+      <c r="C149">
+        <v>9</v>
+      </c>
+      <c r="E149" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F149" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
     <row r="150" spans="3:6">
-      <c r="C150">
-        <v>9</v>
-      </c>
-      <c r="E150" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F150" s="3" t="s">
-        <v>87</v>
+      <c r="E150" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F150" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="151" spans="3:6">
       <c r="E151" s="4" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="F151" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="152" spans="3:6">
-      <c r="E152" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F152" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="153" spans="3:6" ht="30">
+    <row r="152" spans="3:6" ht="30">
+      <c r="E152" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F152" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="153" spans="3:6">
       <c r="E153" s="6" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F153" s="7" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
     </row>
     <row r="154" spans="3:6">
-      <c r="E154" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F154" s="7" t="s">
-        <v>14</v>
+      <c r="E154" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F154" s="9" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="155" spans="3:6">
-      <c r="E155" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="F155" s="9" t="s">
-        <v>40</v>
-      </c>
+      <c r="E155" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="F155" s="26"/>
     </row>
     <row r="156" spans="3:6">
-      <c r="E156" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="F156" s="26"/>
-    </row>
-    <row r="157" spans="3:6">
-      <c r="E157" s="10" t="s">
+      <c r="E156" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F157" s="11" t="s">
+      <c r="F156" s="11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="158" spans="3:6" ht="45">
-      <c r="E158" s="22" t="s">
+    <row r="157" spans="3:6" ht="45">
+      <c r="E157" s="22" t="s">
         <v>62</v>
       </c>
+      <c r="F157" s="14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="158" spans="3:6" ht="30">
+      <c r="E158" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="F158" s="14" t="s">
-        <v>63</v>
+        <v>17</v>
       </c>
     </row>
     <row r="159" spans="3:6" ht="30">
-      <c r="E159" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="F159" s="14" t="s">
-        <v>17</v>
+      <c r="E159" s="15"/>
+      <c r="F159" s="5" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="160" spans="3:6" ht="30">
-      <c r="E160" s="15"/>
+      <c r="E160" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="F160" s="5" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="161" spans="5:6" ht="30">
-      <c r="E161" s="12" t="s">
-        <v>67</v>
-      </c>
+      <c r="E161" s="15"/>
       <c r="F161" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="162" spans="5:6" ht="30">
       <c r="E162" s="15"/>
       <c r="F162" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="163" spans="5:6" ht="30">
-      <c r="E163" s="15"/>
-      <c r="F163" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="164" spans="5:6">
-      <c r="E164" s="6" t="s">
+    <row r="163" spans="5:6">
+      <c r="E163" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F164" s="24" t="s">
+      <c r="F163" s="24" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="165" spans="5:6" ht="60">
-      <c r="E165" s="17" t="s">
+    <row r="164" spans="5:6" ht="60">
+      <c r="E164" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="F165" s="5" t="s">
+      <c r="F164" s="5" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="166" spans="5:6" ht="105.75" thickBot="1">
-      <c r="E166" s="18" t="s">
+    <row r="165" spans="5:6" ht="105.75" thickBot="1">
+      <c r="E165" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="F166" s="23" t="s">
+      <c r="F165" s="23" t="s">
         <v>35</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="E118:F118"/>
-    <mergeCell ref="E137:F137"/>
-    <mergeCell ref="E156:F156"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="E62:F62"/>
-    <mergeCell ref="E78:F78"/>
-    <mergeCell ref="E98:F98"/>
+    <mergeCell ref="E117:F117"/>
+    <mergeCell ref="E136:F136"/>
+    <mergeCell ref="E155:F155"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="E61:F61"/>
+    <mergeCell ref="E77:F77"/>
+    <mergeCell ref="E97:F97"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>